<commit_message>
add remaining kitchens' items to kitchen template
</commit_message>
<xml_diff>
--- a/printer/templates/kitchen.xlsx
+++ b/printer/templates/kitchen.xlsx
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="__Data__">Sheet1!$1:$1048576</definedName>
     <definedName name="__Items__">Sheet1!$8:$8</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$64</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$69</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$7:$7</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Configuration Sheet</t>
   </si>
@@ -125,13 +125,31 @@
   </si>
   <si>
     <t>{{Note}}</t>
+  </si>
+  <si>
+    <t>{{ItemsCountInfo}}</t>
+  </si>
+  <si>
+    <t>{{EditedItemsCountInfo}}</t>
+  </si>
+  <si>
+    <t>{{OtherKitchensTitle}}</t>
+  </si>
+  <si>
+    <t>{{OtherKitchensItemsInfo.Title}}</t>
+  </si>
+  <si>
+    <t>{{OtherKitchensItemsInfo.Value}}</t>
+  </si>
+  <si>
+    <t>{{OtherKitchensItemsCountInfo}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -190,12 +208,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color rgb="FF40485B"/>
-      <name val="Tajawal Medium"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <name val="Vazir"/>
     </font>
@@ -501,7 +513,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
@@ -531,8 +543,62 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1" readingOrder="2"/>
@@ -543,51 +609,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -600,23 +627,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -991,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="130" zoomScaleNormal="145" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:G13"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="160" zoomScaleNormal="145" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1011,78 +1029,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="54.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:7" ht="27.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="23" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="24"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" ht="28.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="26" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="28"/>
+      <c r="G3" s="22"/>
     </row>
     <row r="4" spans="1:7" ht="28.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="40"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="30"/>
     </row>
     <row r="5" spans="1:7" ht="26.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="18" t="s">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="19"/>
+      <c r="G5" s="36"/>
     </row>
     <row r="6" spans="1:7" ht="26.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="32" t="s">
+      <c r="B6" s="24"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="34" t="s">
+      <c r="E6" s="38"/>
+      <c r="F6" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="35"/>
+      <c r="G6" s="40"/>
     </row>
     <row r="7" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
@@ -1097,108 +1115,126 @@
       <c r="A8" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="16"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="34"/>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
+      <c r="A9" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-    </row>
-    <row r="11" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+    </row>
+    <row r="12" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B12" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="16"/>
-    </row>
-    <row r="12" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="34"/>
     </row>
     <row r="13" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+    </row>
+    <row r="14" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+    </row>
+    <row r="15" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="34"/>
+    </row>
+    <row r="16" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+    </row>
+    <row r="17" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-    </row>
-    <row r="14" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-    </row>
-    <row r="15" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-    </row>
-    <row r="16" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-    </row>
-    <row r="17" spans="1:6" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="1:6" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-    </row>
-    <row r="19" spans="1:6" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+    </row>
+    <row r="19" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -1206,7 +1242,7 @@
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="1:6" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
@@ -1214,7 +1250,7 @@
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
     </row>
-    <row r="21" spans="1:6" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -1222,24 +1258,69 @@
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="1:6" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:6" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+    </row>
+    <row r="26" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="A10:G10"/>
+  <mergeCells count="21">
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="A11:G11"/>
     <mergeCell ref="B8:G8"/>
     <mergeCell ref="F5:G5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="A16:G16"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:C6"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="F4:G4"/>
   </mergeCells>

</xml_diff>

<commit_message>
add OtherKitchensInfo for multi-line support
</commit_message>
<xml_diff>
--- a/printer/templates/kitchen.xlsx
+++ b/printer/templates/kitchen.xlsx
@@ -133,9 +133,6 @@
     <t>{{EditedItemsCountInfo}}</t>
   </si>
   <si>
-    <t>{{OtherKitchensTitle}}</t>
-  </si>
-  <si>
     <t>{{OtherKitchensItemsInfo.Title}}</t>
   </si>
   <si>
@@ -143,6 +140,9 @@
   </si>
   <si>
     <t>{{OtherKitchensItemsCountInfo}}</t>
+  </si>
+  <si>
+    <t>{{OtherKitchensInfo.Title}}</t>
   </si>
 </sst>
 </file>
@@ -513,7 +513,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
@@ -546,6 +546,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -609,6 +612,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -630,11 +636,8 @@
     <xf numFmtId="4" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1012,7 +1015,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="160" zoomScaleNormal="145" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:G9"/>
+      <selection activeCell="A14" sqref="A14:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1029,78 +1032,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="54.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="16"/>
+      <c r="A1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" ht="27.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="17" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="18"/>
+      <c r="G2" s="19"/>
     </row>
     <row r="3" spans="1:7" ht="28.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="20" t="s">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="22"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="1:7" ht="28.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="30"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="31"/>
     </row>
     <row r="5" spans="1:7" ht="26.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="35" t="s">
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="36"/>
+      <c r="G5" s="38"/>
     </row>
     <row r="6" spans="1:7" ht="26.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="37" t="s">
+      <c r="B6" s="25"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="38"/>
-      <c r="F6" s="39" t="s">
+      <c r="E6" s="40"/>
+      <c r="F6" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="40"/>
+      <c r="G6" s="42"/>
     </row>
     <row r="7" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
@@ -1115,25 +1118,25 @@
       <c r="A8" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="35"/>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
@@ -1145,74 +1148,74 @@
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
     </row>
     <row r="12" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="35"/>
     </row>
     <row r="13" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
     </row>
     <row r="14" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+    </row>
+    <row r="15" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-    </row>
-    <row r="15" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+    </row>
+    <row r="16" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="34"/>
-    </row>
-    <row r="16" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
     </row>
     <row r="17" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
@@ -1224,15 +1227,15 @@
       <c r="G17" s="13"/>
     </row>
     <row r="18" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
     </row>
     <row r="19" spans="1:7" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>

</xml_diff>